<commit_message>
Update water quality data columns for 2019 and 2020
</commit_message>
<xml_diff>
--- a/References/Jadual-2-3-sungai-tercemar-2020.xlsx
+++ b/References/Jadual-2-3-sungai-tercemar-2020.xlsx
@@ -456,32 +456,32 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>2016-IKA/WQI</t>
+          <t>2019-IKA/WQI</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>2016-category</t>
+          <t>2019-category</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>2016-class</t>
+          <t>2019-class</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>2017-IKA/WQI</t>
+          <t>2020-IKA/WQI</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>2017-category</t>
+          <t>2020-category</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>2017-class</t>
+          <t>2020-class</t>
         </is>
       </c>
     </row>

</xml_diff>